<commit_message>
proje exceline Title verisi eklendi
</commit_message>
<xml_diff>
--- a/files/projects/excel/project_descriptions.XLSX
+++ b/files/projects/excel/project_descriptions.XLSX
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akif\Desktop\streamlit-portfolio\files\projects\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFCF9D38-A532-4366-90B3-4E458B6BE849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2429F829-773C-478B-A8A9-B8CC93BE992C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5352" yWindow="2088" windowWidth="13596" windowHeight="9588" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -25,18 +25,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t>It's a web app that suggests films from a category that user's selected</t>
-  </si>
-  <si>
     <t>Paths</t>
   </si>
   <si>
     <t>../files/projects/photos/film_suggestion_web_app.png</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Film Suggestion App</t>
+  </si>
+  <si>
+    <t>It's a streamlit web app that suggests films from a category that user's selected</t>
   </si>
 </sst>
 </file>
@@ -354,32 +360,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="57.77734375" customWidth="1"/>
-    <col min="2" max="2" width="45" customWidth="1"/>
+    <col min="2" max="2" width="66.88671875" customWidth="1"/>
+    <col min="3" max="3" width="45.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
project.py'a app link kısmı eklendi, excel dosyası değiştirildi
</commit_message>
<xml_diff>
--- a/files/projects/excel/project_descriptions.XLSX
+++ b/files/projects/excel/project_descriptions.XLSX
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akif\Desktop\streamlit-portfolio\files\projects\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E710F2B-4B78-447D-BA17-F63B84765BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D24B6A0F-6319-48C1-87E4-1A14C0E895F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Description</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>files/projects/photos/film_suggestion_web_app.png</t>
+  </si>
+  <si>
+    <t>Links</t>
+  </si>
+  <si>
+    <t>https://film-oneri.streamlit.app/</t>
   </si>
 </sst>
 </file>
@@ -360,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -371,9 +377,10 @@
     <col min="1" max="1" width="57.77734375" customWidth="1"/>
     <col min="2" max="2" width="66.88671875" customWidth="1"/>
     <col min="3" max="3" width="45.5546875" customWidth="1"/>
+    <col min="4" max="4" width="27.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -383,8 +390,11 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -393,6 +403,9 @@
       </c>
       <c r="C2" t="s">
         <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>